<commit_message>
LÇist 03 - aula 05
</commit_message>
<xml_diff>
--- a/Docs/Lista03.xlsx
+++ b/Docs/Lista03.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\curso-excel\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\curso-excel\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54091079-67F0-481A-B855-E5551C81E7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1435B21-7865-484B-96A5-C601321C1257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exerc1" sheetId="1" r:id="rId1"/>
     <sheet name="Exerc2" sheetId="2" r:id="rId2"/>
+    <sheet name="Vendedores" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Produto dos desvios:</t>
   </si>
@@ -90,9 +91,6 @@
     <t>Desvios Y</t>
   </si>
   <si>
-    <t>Contage: X &gt; 2,8</t>
-  </si>
-  <si>
     <t>Tabela Frequência de Y</t>
   </si>
   <si>
@@ -109,17 +107,171 @@
   </si>
   <si>
     <t>Soma dos Quadrados de X</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Tratamento</t>
+  </si>
+  <si>
+    <t>Média Y</t>
+  </si>
+  <si>
+    <t>Média X</t>
+  </si>
+  <si>
+    <t>Soma dos Quadrados de Y</t>
+  </si>
+  <si>
+    <t>Tabela de Médias</t>
+  </si>
+  <si>
+    <t>Filial</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Cimento Portland CP II</t>
+  </si>
+  <si>
+    <t>Areia Fina</t>
+  </si>
+  <si>
+    <t>Brita 1</t>
+  </si>
+  <si>
+    <t>Tijolo Baiano</t>
+  </si>
+  <si>
+    <t>Bloco de Concreto</t>
+  </si>
+  <si>
+    <t>Vergalhão de Aço CA-50</t>
+  </si>
+  <si>
+    <t>Tubo de PVC</t>
+  </si>
+  <si>
+    <t>Argamassa AC I</t>
+  </si>
+  <si>
+    <t>Telha de Cerâmica</t>
+  </si>
+  <si>
+    <t>Massa Corrida</t>
+  </si>
+  <si>
+    <t>Tintas Acrílicas</t>
+  </si>
+  <si>
+    <t>Parafuso para Drywall</t>
+  </si>
+  <si>
+    <t>Fita Isolante</t>
+  </si>
+  <si>
+    <t>Interruptor Simples</t>
+  </si>
+  <si>
+    <t>Tomada 2P+T</t>
+  </si>
+  <si>
+    <t>Porta de Madeira</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t>Saco de 20 kg</t>
+  </si>
+  <si>
+    <t>50 kg</t>
+  </si>
+  <si>
+    <t>9 x 19 x 29 cm</t>
+  </si>
+  <si>
+    <t>14 x 19 x 39 cm</t>
+  </si>
+  <si>
+    <t>8 mm x 12 m</t>
+  </si>
+  <si>
+    <t>100 mm x 6 m</t>
+  </si>
+  <si>
+    <t>Colonial</t>
+  </si>
+  <si>
+    <t>Balde de 18 litros</t>
+  </si>
+  <si>
+    <t>Caixa com 1000 unidades</t>
+  </si>
+  <si>
+    <t>Rolo de 20 metros</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>80 x 210 cm</t>
+  </si>
+  <si>
+    <t>Nome vendedor</t>
+  </si>
+  <si>
+    <t>Sobrenome vendedor</t>
+  </si>
+  <si>
+    <t>Nome;Sobrenome;Filial;Telefone</t>
+  </si>
+  <si>
+    <t>Lúcia;Ferreira;Diadema;(011) 99872-2899</t>
+  </si>
+  <si>
+    <t>Justino;Durão;Mogi Das Cruzes;(011) 99705-6544</t>
+  </si>
+  <si>
+    <t>Cesar;Genesio;Jundiai;(011) 98852-9603</t>
+  </si>
+  <si>
+    <t>Ofélia;Rebolsas;Mogi Das Cruzes;(011) 99705-3977</t>
+  </si>
+  <si>
+    <t>Pedro;Canela;Jundiai;(011) 98852-8316</t>
+  </si>
+  <si>
+    <t>Benedito;Fisher;Diadema;(011) 99872-3150</t>
+  </si>
+  <si>
+    <t>Isolina;Palito;Jundiai;(011) 99705-5953</t>
+  </si>
+  <si>
+    <t>Dario;Pacheco;Jundiai;(011) 98852-9338</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$R$-416]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$R$-416]&quot; &quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +307,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +323,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -227,6 +386,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -239,24 +413,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -595,305 +778,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="A17:D17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.296875" customWidth="1"/>
-    <col min="2" max="5" width="8.3984375" customWidth="1"/>
-    <col min="6" max="6" width="16.8984375" customWidth="1"/>
-    <col min="7" max="7" width="5.59765625" customWidth="1"/>
-    <col min="8" max="8" width="7.3984375" customWidth="1"/>
-    <col min="9" max="1026" width="8.3984375" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.375" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="6" max="6" width="11.75" customWidth="1"/>
+    <col min="7" max="7" width="7.125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="9.375" customWidth="1"/>
+    <col min="10" max="1026" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
         <v>2.92</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="1">
         <v>14.1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
         <v>2.75</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="1">
         <v>15.08</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
         <v>2.78</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="1">
         <v>16.899999999999999</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
         <v>2.73</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="1">
         <v>13.5</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="1">
         <v>14.57</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
         <v>2.89</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="1">
         <v>16</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
         <v>2.98</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="1">
         <v>9.4</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
         <v>2.78</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="1">
         <v>15.66</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
         <v>2.3199999999999998</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="1">
         <v>10.76</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1">
         <v>2.87</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="1">
         <v>13.94</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="G22">
         <v>13</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>11</v>
-      </c>
-      <c r="B22">
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>13</v>
-      </c>
-      <c r="B23">
+      <c r="G23">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24">
         <v>15</v>
       </c>
-      <c r="B24">
+      <c r="G24">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
         <v>17</v>
       </c>
-      <c r="B25" s="7">
+      <c r="G25" s="2">
         <v>19</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.78740157480314954" right="0.78740157480314954" top="1.2791338582677163" bottom="1.2791338582677163" header="0.98385826771653528" footer="0.98385826771653528"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -903,15 +1128,227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" t="str">
+        <f>IFERROR(VLOOKUP(D18,Vendedores!#REF!,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -919,4 +1356,63 @@
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F9143-8FD7-453F-86EE-04F81911DBD8}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>